<commit_message>
filtros con atributos en web
</commit_message>
<xml_diff>
--- a/docs/Productos.xlsx
+++ b/docs/Productos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Paginas_web\kunanmi\Kunanmi_V1\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60933EDC-E64A-40A8-82B4-DD72070FF92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE22B58-D755-4932-9C9F-0A3610B54AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="0" windowWidth="9540" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Avance" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Avance!$A$1:$O$259</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$G$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2190,12 +2191,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2214,6 +2209,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2501,23 +2502,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:O259"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="D264" sqref="D264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.44140625" customWidth="1"/>
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="55.88671875" customWidth="1"/>
-    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11.44140625"/>
     <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="23.88671875" customWidth="1"/>
@@ -2855,99 +2857,99 @@
       <c r="O10" s="30"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="44" t="s">
         <v>476</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="45" t="s">
         <v>478</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="44" t="s">
         <v>203</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46">
+      <c r="E11" s="44"/>
+      <c r="F11" s="44">
         <v>16</v>
       </c>
-      <c r="G11" s="46">
-        <v>10</v>
-      </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46" t="s">
+      <c r="G11" s="44">
+        <v>10</v>
+      </c>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="46"/>
-      <c r="O11" s="46"/>
-    </row>
-    <row r="12" spans="1:15" s="50" customFormat="1" ht="15" thickBot="1">
-      <c r="A12" s="48" t="s">
+      <c r="L11" s="44"/>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+    </row>
+    <row r="12" spans="1:15" s="48" customFormat="1" ht="15" thickBot="1">
+      <c r="A12" s="46" t="s">
         <v>476</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="47" t="s">
         <v>478</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="D12" s="48" t="s">
+      <c r="D12" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48">
+      <c r="E12" s="46"/>
+      <c r="F12" s="46">
         <v>16</v>
       </c>
-      <c r="G12" s="48">
-        <v>10</v>
-      </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48" t="s">
+      <c r="G12" s="46">
+        <v>10</v>
+      </c>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="L12" s="48" t="s">
+      <c r="L12" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
+      <c r="M12" s="46"/>
+      <c r="N12" s="46"/>
+      <c r="O12" s="46"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="42" t="s">
         <v>476</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="43" t="s">
         <v>478</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44">
+      <c r="E13" s="42"/>
+      <c r="F13" s="42">
         <v>16</v>
       </c>
-      <c r="G13" s="44">
-        <v>10</v>
-      </c>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44" t="s">
+      <c r="G13" s="42">
+        <v>10</v>
+      </c>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42" t="s">
         <v>206</v>
       </c>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
+      <c r="L13" s="42"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42"/>
+      <c r="O13" s="42"/>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="30" t="s">
@@ -3210,7 +3212,7 @@
       </c>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="28.8">
       <c r="A22" s="31" t="s">
         <v>476</v>
       </c>
@@ -3441,7 +3443,7 @@
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" hidden="1">
       <c r="A29" s="31" t="s">
         <v>475</v>
       </c>
@@ -3470,7 +3472,7 @@
       <c r="N29" s="30"/>
       <c r="O29" s="30"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" hidden="1">
       <c r="A30" s="31" t="s">
         <v>475</v>
       </c>
@@ -3505,7 +3507,7 @@
       </c>
       <c r="O30" s="30"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" hidden="1">
       <c r="A31" s="31" t="s">
         <v>475</v>
       </c>
@@ -3540,7 +3542,7 @@
       </c>
       <c r="O31" s="30"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" hidden="1">
       <c r="A32" s="31" t="s">
         <v>475</v>
       </c>
@@ -3569,7 +3571,7 @@
       <c r="N32" s="30"/>
       <c r="O32" s="30"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" hidden="1">
       <c r="A33" s="31" t="s">
         <v>475</v>
       </c>
@@ -3600,7 +3602,7 @@
       </c>
       <c r="O33" s="30"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" hidden="1">
       <c r="A34" s="31" t="s">
         <v>475</v>
       </c>
@@ -3631,7 +3633,7 @@
       </c>
       <c r="O34" s="30"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" hidden="1">
       <c r="A35" s="31" t="s">
         <v>475</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" hidden="1">
       <c r="A36" s="31" t="s">
         <v>475</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" hidden="1">
       <c r="A37" s="31" t="s">
         <v>475</v>
       </c>
@@ -3732,7 +3734,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" hidden="1">
       <c r="A38" s="31" t="s">
         <v>475</v>
       </c>
@@ -3767,7 +3769,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" hidden="1">
       <c r="A39" s="31" t="s">
         <v>475</v>
       </c>
@@ -3794,7 +3796,7 @@
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" hidden="1">
       <c r="A40" s="31" t="s">
         <v>475</v>
       </c>
@@ -3821,7 +3823,7 @@
       <c r="N40" s="30"/>
       <c r="O40" s="30"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" hidden="1">
       <c r="A41" s="31" t="s">
         <v>475</v>
       </c>
@@ -3848,7 +3850,7 @@
       <c r="N41" s="30"/>
       <c r="O41" s="30"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" hidden="1">
       <c r="A42" s="31" t="s">
         <v>475</v>
       </c>
@@ -3875,7 +3877,7 @@
       <c r="N42" s="30"/>
       <c r="O42" s="30"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" hidden="1">
       <c r="A43" s="31" t="s">
         <v>475</v>
       </c>
@@ -3902,7 +3904,7 @@
       <c r="N43" s="30"/>
       <c r="O43" s="30"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" hidden="1">
       <c r="A44" s="31" t="s">
         <v>475</v>
       </c>
@@ -3931,7 +3933,7 @@
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" hidden="1">
       <c r="A45" s="31" t="s">
         <v>475</v>
       </c>
@@ -3960,7 +3962,7 @@
       <c r="N45" s="30"/>
       <c r="O45" s="30"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" hidden="1">
       <c r="A46" s="31" t="s">
         <v>475</v>
       </c>
@@ -3989,7 +3991,7 @@
       <c r="N46" s="30"/>
       <c r="O46" s="30"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" hidden="1">
       <c r="A47" s="31" t="s">
         <v>475</v>
       </c>
@@ -4018,7 +4020,7 @@
       <c r="N47" s="30"/>
       <c r="O47" s="30"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" hidden="1">
       <c r="A48" s="31" t="s">
         <v>477</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" hidden="1">
       <c r="A49" s="31" t="s">
         <v>477</v>
       </c>
@@ -4085,7 +4087,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" hidden="1">
       <c r="A50" s="31" t="s">
         <v>477</v>
       </c>
@@ -4120,7 +4122,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" hidden="1">
       <c r="A51" s="31" t="s">
         <v>477</v>
       </c>
@@ -4155,7 +4157,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" hidden="1">
       <c r="A52" s="31" t="s">
         <v>477</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" hidden="1">
       <c r="A53" s="31" t="s">
         <v>477</v>
       </c>
@@ -4227,7 +4229,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" hidden="1">
       <c r="A54" s="31" t="s">
         <v>477</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" hidden="1">
       <c r="A55" s="31" t="s">
         <v>477</v>
       </c>
@@ -4297,7 +4299,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" hidden="1">
       <c r="A56" s="31" t="s">
         <v>477</v>
       </c>
@@ -4334,7 +4336,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" hidden="1">
       <c r="A57" s="31" t="s">
         <v>477</v>
       </c>
@@ -4367,7 +4369,7 @@
       <c r="N57" s="30"/>
       <c r="O57" s="30"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" hidden="1">
       <c r="A58" s="31" t="s">
         <v>477</v>
       </c>
@@ -4400,7 +4402,7 @@
       <c r="N58" s="30"/>
       <c r="O58" s="30"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" hidden="1">
       <c r="A59" s="31" t="s">
         <v>477</v>
       </c>
@@ -4433,7 +4435,7 @@
       <c r="N59" s="30"/>
       <c r="O59" s="30"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" hidden="1">
       <c r="A60" s="31" t="s">
         <v>477</v>
       </c>
@@ -4468,7 +4470,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" hidden="1">
       <c r="A61" s="31" t="s">
         <v>477</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" hidden="1">
       <c r="A62" s="31" t="s">
         <v>477</v>
       </c>
@@ -4542,7 +4544,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" hidden="1">
       <c r="A63" s="31" t="s">
         <v>477</v>
       </c>
@@ -4579,7 +4581,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" hidden="1">
       <c r="A64" s="31" t="s">
         <v>477</v>
       </c>
@@ -4616,7 +4618,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" hidden="1">
       <c r="A65" s="31" t="s">
         <v>477</v>
       </c>
@@ -4653,7 +4655,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" hidden="1">
       <c r="A66" s="31" t="s">
         <v>477</v>
       </c>
@@ -4690,7 +4692,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" hidden="1">
       <c r="A67" s="31" t="s">
         <v>477</v>
       </c>
@@ -4727,7 +4729,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" hidden="1">
       <c r="A68" s="31" t="s">
         <v>477</v>
       </c>
@@ -4764,7 +4766,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" hidden="1">
       <c r="A69" s="31" t="s">
         <v>477</v>
       </c>
@@ -4801,7 +4803,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" hidden="1">
       <c r="A70" s="31" t="s">
         <v>477</v>
       </c>
@@ -4838,7 +4840,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" hidden="1">
       <c r="A71" s="31" t="s">
         <v>477</v>
       </c>
@@ -4875,7 +4877,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" hidden="1">
       <c r="A72" s="31" t="s">
         <v>477</v>
       </c>
@@ -4912,7 +4914,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" hidden="1">
       <c r="A73" s="31" t="s">
         <v>477</v>
       </c>
@@ -4949,7 +4951,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" hidden="1">
       <c r="A74" s="31" t="s">
         <v>477</v>
       </c>
@@ -4986,7 +4988,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" hidden="1">
       <c r="A75" s="31" t="s">
         <v>477</v>
       </c>
@@ -5021,7 +5023,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" hidden="1">
       <c r="A76" s="31" t="s">
         <v>477</v>
       </c>
@@ -5058,7 +5060,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" hidden="1">
       <c r="A77" s="31" t="s">
         <v>477</v>
       </c>
@@ -5093,7 +5095,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" hidden="1">
       <c r="A78" s="31" t="s">
         <v>477</v>
       </c>
@@ -5130,7 +5132,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" hidden="1">
       <c r="A79" s="31" t="s">
         <v>477</v>
       </c>
@@ -5167,7 +5169,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" hidden="1">
       <c r="A80" s="31" t="s">
         <v>477</v>
       </c>
@@ -5204,7 +5206,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" hidden="1">
       <c r="A81" s="31" t="s">
         <v>477</v>
       </c>
@@ -5241,7 +5243,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" hidden="1">
       <c r="A82" s="31" t="s">
         <v>477</v>
       </c>
@@ -5278,7 +5280,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" hidden="1">
       <c r="A83" s="31" t="s">
         <v>477</v>
       </c>
@@ -5315,7 +5317,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" hidden="1">
       <c r="A84" s="31" t="s">
         <v>477</v>
       </c>
@@ -5348,7 +5350,7 @@
       <c r="N84" s="30"/>
       <c r="O84" s="30"/>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" hidden="1">
       <c r="A85" s="31" t="s">
         <v>477</v>
       </c>
@@ -5381,7 +5383,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" hidden="1">
       <c r="A86" s="31" t="s">
         <v>477</v>
       </c>
@@ -5414,7 +5416,7 @@
       <c r="N86" s="30"/>
       <c r="O86" s="30"/>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" hidden="1">
       <c r="A87" s="31" t="s">
         <v>477</v>
       </c>
@@ -5445,7 +5447,7 @@
       <c r="N87" s="30"/>
       <c r="O87" s="30"/>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" hidden="1">
       <c r="A88" s="31" t="s">
         <v>477</v>
       </c>
@@ -5476,7 +5478,7 @@
       <c r="N88" s="30"/>
       <c r="O88" s="30"/>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" hidden="1">
       <c r="A89" s="31" t="s">
         <v>477</v>
       </c>
@@ -5505,7 +5507,7 @@
       <c r="N89" s="30"/>
       <c r="O89" s="30"/>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" hidden="1">
       <c r="A90" s="31" t="s">
         <v>477</v>
       </c>
@@ -5534,7 +5536,7 @@
       <c r="N90" s="30"/>
       <c r="O90" s="30"/>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" hidden="1">
       <c r="A91" s="31" t="s">
         <v>477</v>
       </c>
@@ -5563,7 +5565,7 @@
       <c r="N91" s="30"/>
       <c r="O91" s="30"/>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" hidden="1">
       <c r="A92" s="31" t="s">
         <v>477</v>
       </c>
@@ -5592,7 +5594,7 @@
       <c r="N92" s="30"/>
       <c r="O92" s="30"/>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" hidden="1">
       <c r="A93" s="31" t="s">
         <v>477</v>
       </c>
@@ -5621,7 +5623,7 @@
       <c r="N93" s="30"/>
       <c r="O93" s="30"/>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" hidden="1">
       <c r="A94" s="31" t="s">
         <v>477</v>
       </c>
@@ -5650,7 +5652,7 @@
       <c r="N94" s="30"/>
       <c r="O94" s="30"/>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" hidden="1">
       <c r="A95" s="31" t="s">
         <v>477</v>
       </c>
@@ -5681,7 +5683,7 @@
       <c r="N95" s="30"/>
       <c r="O95" s="30"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" hidden="1">
       <c r="A96" s="31" t="s">
         <v>477</v>
       </c>
@@ -5712,7 +5714,7 @@
       <c r="N96" s="30"/>
       <c r="O96" s="30"/>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" hidden="1">
       <c r="A97" s="31" t="s">
         <v>477</v>
       </c>
@@ -5743,7 +5745,7 @@
       <c r="N97" s="30"/>
       <c r="O97" s="30"/>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" hidden="1">
       <c r="A98" s="31" t="s">
         <v>477</v>
       </c>
@@ -5774,7 +5776,7 @@
       <c r="N98" s="30"/>
       <c r="O98" s="30"/>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" hidden="1">
       <c r="A99" s="31" t="s">
         <v>477</v>
       </c>
@@ -5805,7 +5807,7 @@
       <c r="N99" s="30"/>
       <c r="O99" s="30"/>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" hidden="1">
       <c r="A100" s="31" t="s">
         <v>477</v>
       </c>
@@ -5836,7 +5838,7 @@
       <c r="N100" s="30"/>
       <c r="O100" s="30"/>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" hidden="1">
       <c r="A101" s="31" t="s">
         <v>477</v>
       </c>
@@ -5867,7 +5869,7 @@
       <c r="N101" s="30"/>
       <c r="O101" s="30"/>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" hidden="1">
       <c r="A102" s="31" t="s">
         <v>477</v>
       </c>
@@ -5898,7 +5900,7 @@
       <c r="N102" s="30"/>
       <c r="O102" s="30"/>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" ht="28.8" hidden="1">
       <c r="A103" s="31" t="s">
         <v>477</v>
       </c>
@@ -5929,7 +5931,7 @@
       <c r="N103" s="30"/>
       <c r="O103" s="30"/>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" ht="28.8" hidden="1">
       <c r="A104" s="31" t="s">
         <v>477</v>
       </c>
@@ -5960,7 +5962,7 @@
       <c r="N104" s="30"/>
       <c r="O104" s="30"/>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" ht="28.8" hidden="1">
       <c r="A105" s="31" t="s">
         <v>477</v>
       </c>
@@ -5991,7 +5993,7 @@
       <c r="N105" s="30"/>
       <c r="O105" s="30"/>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" ht="28.8" hidden="1">
       <c r="A106" s="31" t="s">
         <v>477</v>
       </c>
@@ -6022,7 +6024,7 @@
       <c r="N106" s="30"/>
       <c r="O106" s="30"/>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" ht="28.8" hidden="1">
       <c r="A107" s="31" t="s">
         <v>477</v>
       </c>
@@ -6053,7 +6055,7 @@
       <c r="N107" s="30"/>
       <c r="O107" s="30"/>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" ht="28.8" hidden="1">
       <c r="A108" s="31" t="s">
         <v>477</v>
       </c>
@@ -6084,7 +6086,7 @@
       <c r="N108" s="30"/>
       <c r="O108" s="30"/>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" hidden="1">
       <c r="A109" s="31" t="s">
         <v>477</v>
       </c>
@@ -6113,7 +6115,7 @@
       <c r="N109" s="30"/>
       <c r="O109" s="30"/>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" hidden="1">
       <c r="A110" s="31" t="s">
         <v>477</v>
       </c>
@@ -6142,7 +6144,7 @@
       <c r="N110" s="30"/>
       <c r="O110" s="30"/>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" hidden="1">
       <c r="A111" s="31" t="s">
         <v>477</v>
       </c>
@@ -6171,7 +6173,7 @@
       <c r="N111" s="30"/>
       <c r="O111" s="30"/>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" hidden="1">
       <c r="A112" s="31" t="s">
         <v>477</v>
       </c>
@@ -6200,7 +6202,7 @@
       <c r="N112" s="30"/>
       <c r="O112" s="30"/>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" hidden="1">
       <c r="A113" s="31" t="s">
         <v>477</v>
       </c>
@@ -6229,7 +6231,7 @@
       <c r="N113" s="30"/>
       <c r="O113" s="30"/>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" hidden="1">
       <c r="A114" s="31" t="s">
         <v>477</v>
       </c>
@@ -6258,7 +6260,7 @@
       <c r="N114" s="30"/>
       <c r="O114" s="30"/>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" hidden="1">
       <c r="A115" s="31" t="s">
         <v>477</v>
       </c>
@@ -6287,7 +6289,7 @@
       <c r="N115" s="30"/>
       <c r="O115" s="30"/>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" hidden="1">
       <c r="A116" s="31" t="s">
         <v>477</v>
       </c>
@@ -6316,7 +6318,7 @@
       <c r="N116" s="30"/>
       <c r="O116" s="30"/>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" hidden="1">
       <c r="A117" s="31" t="s">
         <v>477</v>
       </c>
@@ -6345,7 +6347,7 @@
       <c r="N117" s="30"/>
       <c r="O117" s="30"/>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" hidden="1">
       <c r="A118" s="31" t="s">
         <v>477</v>
       </c>
@@ -6374,7 +6376,7 @@
       <c r="N118" s="30"/>
       <c r="O118" s="30"/>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" hidden="1">
       <c r="A119" s="31" t="s">
         <v>477</v>
       </c>
@@ -6403,7 +6405,7 @@
       <c r="N119" s="30"/>
       <c r="O119" s="30"/>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" hidden="1">
       <c r="A120" s="31" t="s">
         <v>477</v>
       </c>
@@ -6432,7 +6434,7 @@
       <c r="N120" s="30"/>
       <c r="O120" s="30"/>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" hidden="1">
       <c r="A121" s="31" t="s">
         <v>477</v>
       </c>
@@ -6465,7 +6467,7 @@
       <c r="N121" s="30"/>
       <c r="O121" s="30"/>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" hidden="1">
       <c r="A122" s="31" t="s">
         <v>477</v>
       </c>
@@ -6496,7 +6498,7 @@
       <c r="N122" s="30"/>
       <c r="O122" s="30"/>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" hidden="1">
       <c r="A123" s="31" t="s">
         <v>477</v>
       </c>
@@ -6527,7 +6529,7 @@
       <c r="N123" s="30"/>
       <c r="O123" s="30"/>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" hidden="1">
       <c r="A124" s="31" t="s">
         <v>477</v>
       </c>
@@ -6558,7 +6560,7 @@
       <c r="N124" s="30"/>
       <c r="O124" s="30"/>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" hidden="1">
       <c r="A125" s="31" t="s">
         <v>477</v>
       </c>
@@ -6589,7 +6591,7 @@
       <c r="N125" s="30"/>
       <c r="O125" s="30"/>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" hidden="1">
       <c r="A126" s="31" t="s">
         <v>477</v>
       </c>
@@ -6620,7 +6622,7 @@
       <c r="N126" s="30"/>
       <c r="O126" s="30"/>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" hidden="1">
       <c r="A127" s="31" t="s">
         <v>477</v>
       </c>
@@ -6651,7 +6653,7 @@
       <c r="N127" s="30"/>
       <c r="O127" s="30"/>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" hidden="1">
       <c r="A128" s="31" t="s">
         <v>477</v>
       </c>
@@ -6682,7 +6684,7 @@
       <c r="N128" s="30"/>
       <c r="O128" s="30"/>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" hidden="1">
       <c r="A129" s="31" t="s">
         <v>477</v>
       </c>
@@ -6713,7 +6715,7 @@
       <c r="N129" s="30"/>
       <c r="O129" s="30"/>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" hidden="1">
       <c r="A130" s="31" t="s">
         <v>477</v>
       </c>
@@ -6744,7 +6746,7 @@
       <c r="N130" s="30"/>
       <c r="O130" s="30"/>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" hidden="1">
       <c r="A131" s="31" t="s">
         <v>477</v>
       </c>
@@ -6773,7 +6775,7 @@
       <c r="N131" s="30"/>
       <c r="O131" s="30"/>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" hidden="1">
       <c r="A132" s="31" t="s">
         <v>477</v>
       </c>
@@ -6802,7 +6804,7 @@
       <c r="N132" s="30"/>
       <c r="O132" s="30"/>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" hidden="1">
       <c r="A133" s="31" t="s">
         <v>477</v>
       </c>
@@ -6833,7 +6835,7 @@
       <c r="N133" s="30"/>
       <c r="O133" s="30"/>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" hidden="1">
       <c r="A134" s="31" t="s">
         <v>477</v>
       </c>
@@ -6866,7 +6868,7 @@
       <c r="N134" s="30"/>
       <c r="O134" s="30"/>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" hidden="1">
       <c r="A135" s="31" t="s">
         <v>477</v>
       </c>
@@ -6897,7 +6899,7 @@
       <c r="N135" s="30"/>
       <c r="O135" s="30"/>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" hidden="1">
       <c r="A136" s="31" t="s">
         <v>477</v>
       </c>
@@ -6926,7 +6928,7 @@
       <c r="N136" s="30"/>
       <c r="O136" s="30"/>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" hidden="1">
       <c r="A137" s="31" t="s">
         <v>477</v>
       </c>
@@ -6955,7 +6957,7 @@
       <c r="N137" s="30"/>
       <c r="O137" s="30"/>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" hidden="1">
       <c r="A138" s="31" t="s">
         <v>477</v>
       </c>
@@ -6984,7 +6986,7 @@
       <c r="N138" s="30"/>
       <c r="O138" s="30"/>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" hidden="1">
       <c r="A139" s="31" t="s">
         <v>477</v>
       </c>
@@ -7013,7 +7015,7 @@
       <c r="N139" s="30"/>
       <c r="O139" s="30"/>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" hidden="1">
       <c r="A140" s="31" t="s">
         <v>477</v>
       </c>
@@ -7042,7 +7044,7 @@
       <c r="N140" s="30"/>
       <c r="O140" s="30"/>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" hidden="1">
       <c r="A141" s="31" t="s">
         <v>477</v>
       </c>
@@ -7071,7 +7073,7 @@
       <c r="N141" s="30"/>
       <c r="O141" s="30"/>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" hidden="1">
       <c r="A142" s="31" t="s">
         <v>477</v>
       </c>
@@ -7100,7 +7102,7 @@
       <c r="N142" s="30"/>
       <c r="O142" s="30"/>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" hidden="1">
       <c r="A143" s="31" t="s">
         <v>477</v>
       </c>
@@ -7129,7 +7131,7 @@
       <c r="N143" s="30"/>
       <c r="O143" s="30"/>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" hidden="1">
       <c r="A144" s="31" t="s">
         <v>477</v>
       </c>
@@ -7158,7 +7160,7 @@
       <c r="N144" s="30"/>
       <c r="O144" s="30"/>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" hidden="1">
       <c r="A145" s="31" t="s">
         <v>477</v>
       </c>
@@ -7187,7 +7189,7 @@
       <c r="N145" s="30"/>
       <c r="O145" s="30"/>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" hidden="1">
       <c r="A146" s="31" t="s">
         <v>477</v>
       </c>
@@ -7216,7 +7218,7 @@
       <c r="N146" s="30"/>
       <c r="O146" s="30"/>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" hidden="1">
       <c r="A147" s="31" t="s">
         <v>477</v>
       </c>
@@ -7243,7 +7245,7 @@
       <c r="N147" s="30"/>
       <c r="O147" s="30"/>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" hidden="1">
       <c r="A148" s="31" t="s">
         <v>477</v>
       </c>
@@ -7270,7 +7272,7 @@
       <c r="N148" s="30"/>
       <c r="O148" s="30"/>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" hidden="1">
       <c r="A149" s="31" t="s">
         <v>477</v>
       </c>
@@ -7297,7 +7299,7 @@
       <c r="N149" s="30"/>
       <c r="O149" s="30"/>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" hidden="1">
       <c r="A150" s="31" t="s">
         <v>477</v>
       </c>
@@ -7324,7 +7326,7 @@
       <c r="N150" s="30"/>
       <c r="O150" s="30"/>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" hidden="1">
       <c r="A151" s="31" t="s">
         <v>477</v>
       </c>
@@ -7351,7 +7353,7 @@
       <c r="N151" s="30"/>
       <c r="O151" s="30"/>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" hidden="1">
       <c r="A152" s="31" t="s">
         <v>477</v>
       </c>
@@ -7380,7 +7382,7 @@
       <c r="N152" s="30"/>
       <c r="O152" s="30"/>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" hidden="1">
       <c r="A153" s="31" t="s">
         <v>477</v>
       </c>
@@ -7409,7 +7411,7 @@
       <c r="N153" s="30"/>
       <c r="O153" s="30"/>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" hidden="1">
       <c r="A154" s="31" t="s">
         <v>477</v>
       </c>
@@ -7438,7 +7440,7 @@
       <c r="N154" s="30"/>
       <c r="O154" s="30"/>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" hidden="1">
       <c r="A155" s="31" t="s">
         <v>477</v>
       </c>
@@ -7465,7 +7467,7 @@
       <c r="N155" s="30"/>
       <c r="O155" s="30"/>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" hidden="1">
       <c r="A156" s="31" t="s">
         <v>477</v>
       </c>
@@ -7492,7 +7494,7 @@
       <c r="N156" s="30"/>
       <c r="O156" s="30"/>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" hidden="1">
       <c r="A157" s="31" t="s">
         <v>477</v>
       </c>
@@ -7519,7 +7521,7 @@
       <c r="N157" s="30"/>
       <c r="O157" s="30"/>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" hidden="1">
       <c r="A158" s="31" t="s">
         <v>477</v>
       </c>
@@ -7546,7 +7548,7 @@
       <c r="N158" s="30"/>
       <c r="O158" s="30"/>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" hidden="1">
       <c r="A159" s="31" t="s">
         <v>477</v>
       </c>
@@ -7573,7 +7575,7 @@
       <c r="N159" s="30"/>
       <c r="O159" s="30"/>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" hidden="1">
       <c r="A160" s="31" t="s">
         <v>477</v>
       </c>
@@ -7600,7 +7602,7 @@
       <c r="N160" s="30"/>
       <c r="O160" s="30"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" hidden="1">
       <c r="A161" s="31" t="s">
         <v>477</v>
       </c>
@@ -7627,7 +7629,7 @@
       <c r="N161" s="30"/>
       <c r="O161" s="30"/>
     </row>
-    <row r="162" spans="1:15" ht="13.5" customHeight="1">
+    <row r="162" spans="1:15" ht="13.5" hidden="1" customHeight="1">
       <c r="A162" s="31" t="s">
         <v>477</v>
       </c>
@@ -7656,7 +7658,7 @@
       <c r="N162" s="30"/>
       <c r="O162" s="30"/>
     </row>
-    <row r="163" spans="1:15" ht="13.5" customHeight="1">
+    <row r="163" spans="1:15" ht="13.5" hidden="1" customHeight="1">
       <c r="A163" s="31" t="s">
         <v>477</v>
       </c>
@@ -7683,7 +7685,7 @@
       <c r="N163" s="30"/>
       <c r="O163" s="30"/>
     </row>
-    <row r="164" spans="1:15" ht="13.5" customHeight="1">
+    <row r="164" spans="1:15" ht="13.5" hidden="1" customHeight="1">
       <c r="A164" s="31" t="s">
         <v>477</v>
       </c>
@@ -7710,7 +7712,7 @@
       <c r="N164" s="30"/>
       <c r="O164" s="30"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" hidden="1">
       <c r="A165" s="31" t="s">
         <v>477</v>
       </c>
@@ -7739,7 +7741,7 @@
       <c r="N165" s="30"/>
       <c r="O165" s="30"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" hidden="1">
       <c r="A166" s="31" t="s">
         <v>477</v>
       </c>
@@ -7766,7 +7768,7 @@
       <c r="N166" s="30"/>
       <c r="O166" s="30"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" hidden="1">
       <c r="A167" s="31" t="s">
         <v>477</v>
       </c>
@@ -7793,7 +7795,7 @@
       <c r="N167" s="30"/>
       <c r="O167" s="30"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" hidden="1">
       <c r="A168" s="31" t="s">
         <v>477</v>
       </c>
@@ -7820,7 +7822,7 @@
       <c r="N168" s="30"/>
       <c r="O168" s="30"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" hidden="1">
       <c r="A169" s="31" t="s">
         <v>477</v>
       </c>
@@ -7847,7 +7849,7 @@
       <c r="N169" s="30"/>
       <c r="O169" s="30"/>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" hidden="1">
       <c r="A170" s="31" t="s">
         <v>477</v>
       </c>
@@ -7874,7 +7876,7 @@
       <c r="N170" s="30"/>
       <c r="O170" s="30"/>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" hidden="1">
       <c r="A171" s="31" t="s">
         <v>477</v>
       </c>
@@ -7901,7 +7903,7 @@
       <c r="N171" s="30"/>
       <c r="O171" s="30"/>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" hidden="1">
       <c r="A172" s="31" t="s">
         <v>477</v>
       </c>
@@ -7928,7 +7930,7 @@
       <c r="N172" s="30"/>
       <c r="O172" s="30"/>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" hidden="1">
       <c r="A173" s="31" t="s">
         <v>477</v>
       </c>
@@ -7957,7 +7959,7 @@
       <c r="N173" s="30"/>
       <c r="O173" s="30"/>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:15" hidden="1">
       <c r="A174" s="31" t="s">
         <v>477</v>
       </c>
@@ -7990,7 +7992,7 @@
       <c r="N174" s="30"/>
       <c r="O174" s="30"/>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" hidden="1">
       <c r="A175" s="31" t="s">
         <v>477</v>
       </c>
@@ -8019,7 +8021,7 @@
       <c r="N175" s="30"/>
       <c r="O175" s="30"/>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" hidden="1">
       <c r="A176" s="31" t="s">
         <v>477</v>
       </c>
@@ -8048,7 +8050,7 @@
       <c r="N176" s="30"/>
       <c r="O176" s="30"/>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" hidden="1">
       <c r="A177" s="31" t="s">
         <v>477</v>
       </c>
@@ -8079,7 +8081,7 @@
       <c r="N177" s="30"/>
       <c r="O177" s="30"/>
     </row>
-    <row r="178" spans="1:15">
+    <row r="178" spans="1:15" hidden="1">
       <c r="A178" s="31" t="s">
         <v>477</v>
       </c>
@@ -8110,7 +8112,7 @@
       <c r="N178" s="30"/>
       <c r="O178" s="30"/>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" hidden="1">
       <c r="A179" s="31" t="s">
         <v>477</v>
       </c>
@@ -8141,7 +8143,7 @@
       <c r="N179" s="30"/>
       <c r="O179" s="30"/>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" hidden="1">
       <c r="A180" s="31" t="s">
         <v>477</v>
       </c>
@@ -8172,7 +8174,7 @@
       <c r="N180" s="30"/>
       <c r="O180" s="30"/>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" hidden="1">
       <c r="A181" s="31" t="s">
         <v>477</v>
       </c>
@@ -8203,7 +8205,7 @@
       <c r="N181" s="30"/>
       <c r="O181" s="30"/>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" hidden="1">
       <c r="A182" s="31" t="s">
         <v>477</v>
       </c>
@@ -8234,7 +8236,7 @@
       <c r="N182" s="30"/>
       <c r="O182" s="30"/>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" hidden="1">
       <c r="A183" s="31" t="s">
         <v>477</v>
       </c>
@@ -8265,7 +8267,7 @@
       <c r="N183" s="30"/>
       <c r="O183" s="30"/>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" hidden="1">
       <c r="A184" s="31" t="s">
         <v>477</v>
       </c>
@@ -8296,7 +8298,7 @@
       <c r="N184" s="30"/>
       <c r="O184" s="30"/>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" hidden="1">
       <c r="A185" s="31" t="s">
         <v>477</v>
       </c>
@@ -8327,7 +8329,7 @@
       <c r="N185" s="30"/>
       <c r="O185" s="30"/>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" hidden="1">
       <c r="A186" s="31" t="s">
         <v>477</v>
       </c>
@@ -8358,7 +8360,7 @@
       <c r="N186" s="30"/>
       <c r="O186" s="30"/>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" hidden="1">
       <c r="A187" s="31" t="s">
         <v>477</v>
       </c>
@@ -8389,7 +8391,7 @@
       <c r="N187" s="30"/>
       <c r="O187" s="30"/>
     </row>
-    <row r="188" spans="1:15">
+    <row r="188" spans="1:15" hidden="1">
       <c r="A188" s="31" t="s">
         <v>477</v>
       </c>
@@ -8420,7 +8422,7 @@
       <c r="N188" s="30"/>
       <c r="O188" s="30"/>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" hidden="1">
       <c r="A189" s="31" t="s">
         <v>477</v>
       </c>
@@ -8451,7 +8453,7 @@
       <c r="N189" s="30"/>
       <c r="O189" s="30"/>
     </row>
-    <row r="190" spans="1:15">
+    <row r="190" spans="1:15" hidden="1">
       <c r="A190" s="31" t="s">
         <v>477</v>
       </c>
@@ -8482,7 +8484,7 @@
       <c r="N190" s="30"/>
       <c r="O190" s="30"/>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" hidden="1">
       <c r="A191" s="31" t="s">
         <v>477</v>
       </c>
@@ -8513,7 +8515,7 @@
       <c r="N191" s="30"/>
       <c r="O191" s="30"/>
     </row>
-    <row r="192" spans="1:15">
+    <row r="192" spans="1:15" hidden="1">
       <c r="A192" s="31" t="s">
         <v>477</v>
       </c>
@@ -8544,7 +8546,7 @@
       <c r="N192" s="30"/>
       <c r="O192" s="30"/>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" hidden="1">
       <c r="A193" s="31" t="s">
         <v>477</v>
       </c>
@@ -8575,7 +8577,7 @@
       <c r="N193" s="30"/>
       <c r="O193" s="30"/>
     </row>
-    <row r="194" spans="1:15">
+    <row r="194" spans="1:15" hidden="1">
       <c r="A194" s="31" t="s">
         <v>477</v>
       </c>
@@ -8606,7 +8608,7 @@
       <c r="N194" s="30"/>
       <c r="O194" s="30"/>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" hidden="1">
       <c r="A195" s="31" t="s">
         <v>477</v>
       </c>
@@ -8637,7 +8639,7 @@
       <c r="N195" s="30"/>
       <c r="O195" s="30"/>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" hidden="1">
       <c r="A196" s="31" t="s">
         <v>477</v>
       </c>
@@ -8668,7 +8670,7 @@
       <c r="N196" s="30"/>
       <c r="O196" s="30"/>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" hidden="1">
       <c r="A197" s="31" t="s">
         <v>477</v>
       </c>
@@ -8699,7 +8701,7 @@
       <c r="N197" s="30"/>
       <c r="O197" s="30"/>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" hidden="1">
       <c r="A198" s="31" t="s">
         <v>477</v>
       </c>
@@ -8730,7 +8732,7 @@
       <c r="N198" s="30"/>
       <c r="O198" s="30"/>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" hidden="1">
       <c r="A199" s="31" t="s">
         <v>477</v>
       </c>
@@ -8761,7 +8763,7 @@
       <c r="N199" s="30"/>
       <c r="O199" s="30"/>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" hidden="1">
       <c r="A200" s="31" t="s">
         <v>477</v>
       </c>
@@ -8792,7 +8794,7 @@
       <c r="N200" s="30"/>
       <c r="O200" s="30"/>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" hidden="1">
       <c r="A201" s="31" t="s">
         <v>477</v>
       </c>
@@ -8823,7 +8825,7 @@
       <c r="N201" s="30"/>
       <c r="O201" s="30"/>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" hidden="1">
       <c r="A202" s="31" t="s">
         <v>477</v>
       </c>
@@ -8854,7 +8856,7 @@
       <c r="N202" s="30"/>
       <c r="O202" s="30"/>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" hidden="1">
       <c r="A203" s="31" t="s">
         <v>477</v>
       </c>
@@ -8885,7 +8887,7 @@
       <c r="N203" s="30"/>
       <c r="O203" s="30"/>
     </row>
-    <row r="204" spans="1:15">
+    <row r="204" spans="1:15" hidden="1">
       <c r="A204" s="31" t="s">
         <v>477</v>
       </c>
@@ -8916,7 +8918,7 @@
       <c r="N204" s="30"/>
       <c r="O204" s="30"/>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" hidden="1">
       <c r="A205" s="31" t="s">
         <v>477</v>
       </c>
@@ -8947,7 +8949,7 @@
       <c r="N205" s="30"/>
       <c r="O205" s="30"/>
     </row>
-    <row r="206" spans="1:15">
+    <row r="206" spans="1:15" hidden="1">
       <c r="A206" s="31" t="s">
         <v>477</v>
       </c>
@@ -8978,7 +8980,7 @@
       <c r="N206" s="30"/>
       <c r="O206" s="30"/>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" hidden="1">
       <c r="A207" s="31" t="s">
         <v>477</v>
       </c>
@@ -9009,7 +9011,7 @@
       <c r="N207" s="30"/>
       <c r="O207" s="30"/>
     </row>
-    <row r="208" spans="1:15">
+    <row r="208" spans="1:15" hidden="1">
       <c r="A208" s="31" t="s">
         <v>477</v>
       </c>
@@ -9040,7 +9042,7 @@
       <c r="N208" s="30"/>
       <c r="O208" s="30"/>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" hidden="1">
       <c r="A209" s="31" t="s">
         <v>477</v>
       </c>
@@ -9071,7 +9073,7 @@
       <c r="N209" s="30"/>
       <c r="O209" s="30"/>
     </row>
-    <row r="210" spans="1:15">
+    <row r="210" spans="1:15" hidden="1">
       <c r="A210" s="31" t="s">
         <v>477</v>
       </c>
@@ -9102,7 +9104,7 @@
       <c r="N210" s="30"/>
       <c r="O210" s="30"/>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" hidden="1">
       <c r="A211" s="31" t="s">
         <v>477</v>
       </c>
@@ -9133,7 +9135,7 @@
       <c r="N211" s="30"/>
       <c r="O211" s="30"/>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" hidden="1">
       <c r="A212" s="31" t="s">
         <v>477</v>
       </c>
@@ -9164,7 +9166,7 @@
       <c r="N212" s="30"/>
       <c r="O212" s="30"/>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" hidden="1">
       <c r="A213" s="31" t="s">
         <v>477</v>
       </c>
@@ -9195,7 +9197,7 @@
       <c r="N213" s="30"/>
       <c r="O213" s="30"/>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" hidden="1">
       <c r="A214" s="31" t="s">
         <v>477</v>
       </c>
@@ -9226,7 +9228,7 @@
       <c r="N214" s="30"/>
       <c r="O214" s="30"/>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" hidden="1">
       <c r="A215" s="31" t="s">
         <v>477</v>
       </c>
@@ -9257,7 +9259,7 @@
       <c r="N215" s="30"/>
       <c r="O215" s="30"/>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" hidden="1">
       <c r="A216" s="31" t="s">
         <v>477</v>
       </c>
@@ -9288,7 +9290,7 @@
       <c r="N216" s="30"/>
       <c r="O216" s="30"/>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" hidden="1">
       <c r="A217" s="31" t="s">
         <v>477</v>
       </c>
@@ -9319,7 +9321,7 @@
       <c r="N217" s="30"/>
       <c r="O217" s="30"/>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" hidden="1">
       <c r="A218" s="31" t="s">
         <v>477</v>
       </c>
@@ -9350,7 +9352,7 @@
       <c r="N218" s="30"/>
       <c r="O218" s="30"/>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" hidden="1">
       <c r="A219" s="31" t="s">
         <v>477</v>
       </c>
@@ -9381,7 +9383,7 @@
       <c r="N219" s="30"/>
       <c r="O219" s="30"/>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" hidden="1">
       <c r="A220" s="31" t="s">
         <v>477</v>
       </c>
@@ -9412,7 +9414,7 @@
       <c r="N220" s="30"/>
       <c r="O220" s="30"/>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" hidden="1">
       <c r="A221" s="31" t="s">
         <v>477</v>
       </c>
@@ -9443,7 +9445,7 @@
       <c r="N221" s="30"/>
       <c r="O221" s="30"/>
     </row>
-    <row r="222" spans="1:15">
+    <row r="222" spans="1:15" hidden="1">
       <c r="A222" s="31" t="s">
         <v>477</v>
       </c>
@@ -9474,7 +9476,7 @@
       <c r="N222" s="30"/>
       <c r="O222" s="30"/>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" hidden="1">
       <c r="A223" s="31" t="s">
         <v>477</v>
       </c>
@@ -9505,7 +9507,7 @@
       <c r="N223" s="30"/>
       <c r="O223" s="30"/>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" hidden="1">
       <c r="A224" s="31" t="s">
         <v>477</v>
       </c>
@@ -9536,7 +9538,7 @@
       <c r="N224" s="30"/>
       <c r="O224" s="30"/>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" hidden="1">
       <c r="A225" s="31" t="s">
         <v>477</v>
       </c>
@@ -9567,7 +9569,7 @@
       <c r="N225" s="30"/>
       <c r="O225" s="30"/>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" hidden="1">
       <c r="A226" s="31" t="s">
         <v>477</v>
       </c>
@@ -9598,7 +9600,7 @@
       <c r="N226" s="30"/>
       <c r="O226" s="30"/>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" hidden="1">
       <c r="A227" s="31" t="s">
         <v>477</v>
       </c>
@@ -9629,7 +9631,7 @@
       <c r="N227" s="30"/>
       <c r="O227" s="30"/>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" hidden="1">
       <c r="A228" s="31" t="s">
         <v>477</v>
       </c>
@@ -9660,7 +9662,7 @@
       <c r="N228" s="30"/>
       <c r="O228" s="30"/>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" hidden="1">
       <c r="A229" s="31" t="s">
         <v>477</v>
       </c>
@@ -9691,7 +9693,7 @@
       <c r="N229" s="30"/>
       <c r="O229" s="30"/>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" hidden="1">
       <c r="A230" s="31" t="s">
         <v>477</v>
       </c>
@@ -9722,7 +9724,7 @@
       <c r="N230" s="30"/>
       <c r="O230" s="30"/>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" hidden="1">
       <c r="A231" s="31" t="s">
         <v>477</v>
       </c>
@@ -9753,7 +9755,7 @@
       <c r="N231" s="30"/>
       <c r="O231" s="30"/>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" hidden="1">
       <c r="A232" s="31" t="s">
         <v>477</v>
       </c>
@@ -9784,7 +9786,7 @@
       <c r="N232" s="30"/>
       <c r="O232" s="30"/>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" hidden="1">
       <c r="A233" s="31" t="s">
         <v>477</v>
       </c>
@@ -9815,7 +9817,7 @@
       <c r="N233" s="30"/>
       <c r="O233" s="30"/>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" hidden="1">
       <c r="A234" s="31" t="s">
         <v>477</v>
       </c>
@@ -9846,7 +9848,7 @@
       <c r="N234" s="30"/>
       <c r="O234" s="30"/>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" hidden="1">
       <c r="A235" s="31" t="s">
         <v>477</v>
       </c>
@@ -9877,7 +9879,7 @@
       <c r="N235" s="30"/>
       <c r="O235" s="30"/>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" hidden="1">
       <c r="A236" s="31" t="s">
         <v>477</v>
       </c>
@@ -9908,7 +9910,7 @@
       <c r="N236" s="30"/>
       <c r="O236" s="30"/>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" hidden="1">
       <c r="A237" s="31" t="s">
         <v>477</v>
       </c>
@@ -9939,7 +9941,7 @@
       <c r="N237" s="30"/>
       <c r="O237" s="30"/>
     </row>
-    <row r="238" spans="1:15">
+    <row r="238" spans="1:15" hidden="1">
       <c r="A238" s="31" t="s">
         <v>477</v>
       </c>
@@ -9970,7 +9972,7 @@
       <c r="N238" s="30"/>
       <c r="O238" s="30"/>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" hidden="1">
       <c r="A239" s="31" t="s">
         <v>477</v>
       </c>
@@ -10001,7 +10003,7 @@
       <c r="N239" s="30"/>
       <c r="O239" s="30"/>
     </row>
-    <row r="240" spans="1:15">
+    <row r="240" spans="1:15" hidden="1">
       <c r="A240" s="31" t="s">
         <v>477</v>
       </c>
@@ -10032,7 +10034,7 @@
       <c r="N240" s="30"/>
       <c r="O240" s="30"/>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" hidden="1">
       <c r="A241" s="31" t="s">
         <v>477</v>
       </c>
@@ -10063,7 +10065,7 @@
       <c r="N241" s="30"/>
       <c r="O241" s="30"/>
     </row>
-    <row r="242" spans="1:15">
+    <row r="242" spans="1:15" hidden="1">
       <c r="A242" s="31" t="s">
         <v>477</v>
       </c>
@@ -10094,7 +10096,7 @@
       <c r="N242" s="30"/>
       <c r="O242" s="30"/>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" hidden="1">
       <c r="A243" s="31" t="s">
         <v>477</v>
       </c>
@@ -10125,7 +10127,7 @@
       <c r="N243" s="30"/>
       <c r="O243" s="30"/>
     </row>
-    <row r="244" spans="1:15">
+    <row r="244" spans="1:15" hidden="1">
       <c r="A244" s="31" t="s">
         <v>477</v>
       </c>
@@ -10156,7 +10158,7 @@
       <c r="N244" s="30"/>
       <c r="O244" s="30"/>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" hidden="1">
       <c r="A245" s="31" t="s">
         <v>477</v>
       </c>
@@ -10187,7 +10189,7 @@
       <c r="N245" s="30"/>
       <c r="O245" s="30"/>
     </row>
-    <row r="246" spans="1:15">
+    <row r="246" spans="1:15" hidden="1">
       <c r="A246" s="31" t="s">
         <v>477</v>
       </c>
@@ -10218,7 +10220,7 @@
       <c r="N246" s="30"/>
       <c r="O246" s="30"/>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" hidden="1">
       <c r="A247" s="31" t="s">
         <v>477</v>
       </c>
@@ -10249,7 +10251,7 @@
       <c r="N247" s="30"/>
       <c r="O247" s="30"/>
     </row>
-    <row r="248" spans="1:15">
+    <row r="248" spans="1:15" hidden="1">
       <c r="A248" s="31" t="s">
         <v>477</v>
       </c>
@@ -10280,7 +10282,7 @@
       <c r="N248" s="30"/>
       <c r="O248" s="30"/>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" hidden="1">
       <c r="A249" s="31" t="s">
         <v>477</v>
       </c>
@@ -10311,7 +10313,7 @@
       <c r="N249" s="30"/>
       <c r="O249" s="30"/>
     </row>
-    <row r="250" spans="1:15">
+    <row r="250" spans="1:15" hidden="1">
       <c r="A250" s="31" t="s">
         <v>477</v>
       </c>
@@ -10342,7 +10344,7 @@
       <c r="N250" s="30"/>
       <c r="O250" s="30"/>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" hidden="1">
       <c r="A251" s="31" t="s">
         <v>477</v>
       </c>
@@ -10375,7 +10377,7 @@
       <c r="N251" s="30"/>
       <c r="O251" s="30"/>
     </row>
-    <row r="252" spans="1:15">
+    <row r="252" spans="1:15" hidden="1">
       <c r="A252" s="31" t="s">
         <v>477</v>
       </c>
@@ -10408,7 +10410,7 @@
       <c r="N252" s="30"/>
       <c r="O252" s="30"/>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" hidden="1">
       <c r="A253" s="31" t="s">
         <v>477</v>
       </c>
@@ -10441,7 +10443,7 @@
       <c r="N253" s="30"/>
       <c r="O253" s="30"/>
     </row>
-    <row r="254" spans="1:15">
+    <row r="254" spans="1:15" hidden="1">
       <c r="A254" s="31" t="s">
         <v>477</v>
       </c>
@@ -10474,7 +10476,7 @@
       <c r="N254" s="30"/>
       <c r="O254" s="30"/>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" hidden="1">
       <c r="A255" s="31" t="s">
         <v>477</v>
       </c>
@@ -10507,7 +10509,7 @@
       <c r="N255" s="30"/>
       <c r="O255" s="30"/>
     </row>
-    <row r="256" spans="1:15">
+    <row r="256" spans="1:15" hidden="1">
       <c r="A256" s="31" t="s">
         <v>477</v>
       </c>
@@ -10540,7 +10542,7 @@
       <c r="N256" s="30"/>
       <c r="O256" s="30"/>
     </row>
-    <row r="257" spans="1:15">
+    <row r="257" spans="1:15" hidden="1">
       <c r="A257" s="31" t="s">
         <v>477</v>
       </c>
@@ -10573,7 +10575,7 @@
       <c r="N257" s="30"/>
       <c r="O257" s="30"/>
     </row>
-    <row r="258" spans="1:15" ht="15" customHeight="1">
+    <row r="258" spans="1:15" ht="15" hidden="1" customHeight="1">
       <c r="A258" s="31" t="s">
         <v>477</v>
       </c>
@@ -10606,7 +10608,7 @@
       <c r="N258" s="30"/>
       <c r="O258" s="30"/>
     </row>
-    <row r="259" spans="1:15" ht="16.5" customHeight="1">
+    <row r="259" spans="1:15" ht="16.5" hidden="1" customHeight="1">
       <c r="A259" s="31" t="s">
         <v>477</v>
       </c>
@@ -10640,7 +10642,13 @@
       <c r="O259" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O259" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O259" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Cuidado facial (2)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -10650,9 +10658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C63E3B-0038-4417-BE29-7F9029D8CDB7}">
   <dimension ref="A1:AE97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
@@ -10773,7 +10779,7 @@
       <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="51" t="s">
+      <c r="P3" s="49" t="s">
         <v>544</v>
       </c>
       <c r="R3" t="s">
@@ -10820,7 +10826,7 @@
       <c r="J4" t="s">
         <v>537</v>
       </c>
-      <c r="P4" s="52"/>
+      <c r="P4" s="50"/>
       <c r="R4" t="s">
         <v>436</v>
       </c>
@@ -10847,7 +10853,7 @@
       <c r="J5" t="s">
         <v>301</v>
       </c>
-      <c r="P5" s="52" t="s">
+      <c r="P5" s="50" t="s">
         <v>343</v>
       </c>
       <c r="R5" t="s">
@@ -10876,7 +10882,7 @@
       <c r="J6" t="s">
         <v>538</v>
       </c>
-      <c r="P6" s="52"/>
+      <c r="P6" s="50"/>
       <c r="R6" t="s">
         <v>430</v>
       </c>
@@ -10900,7 +10906,7 @@
       <c r="J7" t="s">
         <v>434</v>
       </c>
-      <c r="P7" s="52" t="s">
+      <c r="P7" s="50" t="s">
         <v>314</v>
       </c>
       <c r="R7" t="s">
@@ -10926,7 +10932,7 @@
       <c r="J8" t="s">
         <v>435</v>
       </c>
-      <c r="P8" s="52"/>
+      <c r="P8" s="50"/>
       <c r="R8" t="s">
         <v>543</v>
       </c>
@@ -10950,7 +10956,7 @@
       <c r="J9" t="s">
         <v>539</v>
       </c>
-      <c r="P9" s="52" t="s">
+      <c r="P9" s="50" t="s">
         <v>315</v>
       </c>
       <c r="R9" t="s">
@@ -10973,7 +10979,7 @@
       <c r="F10" t="str">
         <v>Woodland</v>
       </c>
-      <c r="P10" s="52"/>
+      <c r="P10" s="50"/>
       <c r="R10" t="s">
         <v>44</v>
       </c>
@@ -10994,7 +11000,7 @@
       <c r="F11" t="str">
         <v>Sweetie</v>
       </c>
-      <c r="P11" s="52" t="s">
+      <c r="P11" s="50" t="s">
         <v>316</v>
       </c>
     </row>
@@ -11014,7 +11020,7 @@
       <c r="F12" t="str">
         <v>Citrus</v>
       </c>
-      <c r="P12" s="52"/>
+      <c r="P12" s="50"/>
     </row>
     <row r="13" spans="1:31">
       <c r="B13" t="str">
@@ -11032,7 +11038,7 @@
       <c r="F13" t="str">
         <v>Complex Scents</v>
       </c>
-      <c r="P13" s="52" t="s">
+      <c r="P13" s="50" t="s">
         <v>317</v>
       </c>
     </row>
@@ -11052,7 +11058,7 @@
       <c r="F14" t="str">
         <v>Berries</v>
       </c>
-      <c r="P14" s="52"/>
+      <c r="P14" s="50"/>
     </row>
     <row r="15" spans="1:31">
       <c r="B15" t="str">
@@ -11067,7 +11073,7 @@
       <c r="F15" t="str">
         <v>Herbal &amp; Green</v>
       </c>
-      <c r="P15" s="52" t="s">
+      <c r="P15" s="50" t="s">
         <v>431</v>
       </c>
     </row>
@@ -11092,7 +11098,7 @@
       <c r="D17" t="str">
         <v>Patchouli</v>
       </c>
-      <c r="P17" s="51" t="s">
+      <c r="P17" s="49" t="s">
         <v>545</v>
       </c>
     </row>
@@ -11106,7 +11112,7 @@
       <c r="D18" t="str">
         <v>Rosemary</v>
       </c>
-      <c r="P18" s="52"/>
+      <c r="P18" s="50"/>
     </row>
     <row r="19" spans="2:16">
       <c r="B19" t="str">
@@ -11118,7 +11124,7 @@
       <c r="D19" t="str">
         <v>Palo Santo</v>
       </c>
-      <c r="P19" s="52" t="s">
+      <c r="P19" s="50" t="s">
         <v>346</v>
       </c>
     </row>
@@ -11129,7 +11135,7 @@
       <c r="D20" t="str">
         <v>Sandalwood</v>
       </c>
-      <c r="P20" s="52"/>
+      <c r="P20" s="50"/>
     </row>
     <row r="21" spans="2:16">
       <c r="B21" t="str">
@@ -11138,7 +11144,7 @@
       <c r="D21" t="str">
         <v>Bamboo</v>
       </c>
-      <c r="P21" s="52" t="s">
+      <c r="P21" s="50" t="s">
         <v>349</v>
       </c>
     </row>
@@ -11149,7 +11155,7 @@
       <c r="D22" t="str">
         <v>Eucalyptus</v>
       </c>
-      <c r="P22" s="52"/>
+      <c r="P22" s="50"/>
     </row>
     <row r="23" spans="2:16">
       <c r="B23" t="str">
@@ -11158,7 +11164,7 @@
       <c r="D23" t="str">
         <v>Jassmine</v>
       </c>
-      <c r="P23" s="52" t="s">
+      <c r="P23" s="50" t="s">
         <v>460</v>
       </c>
     </row>
@@ -11169,7 +11175,7 @@
       <c r="D24" t="str">
         <v>Gardenia</v>
       </c>
-      <c r="P24" s="52"/>
+      <c r="P24" s="50"/>
     </row>
     <row r="25" spans="2:16">
       <c r="B25" t="str">
@@ -11178,7 +11184,7 @@
       <c r="D25" t="str">
         <v>Rose Notes</v>
       </c>
-      <c r="P25" s="52" t="s">
+      <c r="P25" s="50" t="s">
         <v>366</v>
       </c>
     </row>
@@ -11186,13 +11192,13 @@
       <c r="D26" t="str">
         <v>Violetta</v>
       </c>
-      <c r="P26" s="52"/>
+      <c r="P26" s="50"/>
     </row>
     <row r="27" spans="2:16">
       <c r="D27" t="str">
         <v>Grape Fruit</v>
       </c>
-      <c r="P27" s="52" t="s">
+      <c r="P27" s="50" t="s">
         <v>318</v>
       </c>
     </row>
@@ -11200,13 +11206,13 @@
       <c r="D28" t="str">
         <v>Bergamot</v>
       </c>
-      <c r="P28" s="52"/>
+      <c r="P28" s="50"/>
     </row>
     <row r="29" spans="2:16">
       <c r="D29" t="str">
         <v>Passion Fruit</v>
       </c>
-      <c r="P29" s="52" t="s">
+      <c r="P29" s="50" t="s">
         <v>319</v>
       </c>
     </row>
@@ -11214,13 +11220,13 @@
       <c r="D30" t="str">
         <v>Lemon Bliss</v>
       </c>
-      <c r="P30" s="52"/>
+      <c r="P30" s="50"/>
     </row>
     <row r="31" spans="2:16">
       <c r="D31" t="str">
         <v>Orange Bliss</v>
       </c>
-      <c r="P31" s="52" t="s">
+      <c r="P31" s="50" t="s">
         <v>320</v>
       </c>
     </row>
@@ -11228,13 +11234,13 @@
       <c r="D32" t="str">
         <v>Citronella</v>
       </c>
-      <c r="P32" s="52"/>
+      <c r="P32" s="50"/>
     </row>
     <row r="33" spans="4:16">
       <c r="D33" t="str">
         <v>Sweet Clementine</v>
       </c>
-      <c r="P33" s="52" t="s">
+      <c r="P33" s="50" t="s">
         <v>321</v>
       </c>
     </row>
@@ -11242,13 +11248,13 @@
       <c r="D34" t="str">
         <v>Floral &amp; Citrus</v>
       </c>
-      <c r="P34" s="52"/>
+      <c r="P34" s="50"/>
     </row>
     <row r="35" spans="4:16">
       <c r="D35" t="str">
         <v>Coconut</v>
       </c>
-      <c r="P35" s="52" t="s">
+      <c r="P35" s="50" t="s">
         <v>322</v>
       </c>
     </row>
@@ -11256,13 +11262,13 @@
       <c r="D36" t="str">
         <v>Vanilla Latte</v>
       </c>
-      <c r="P36" s="52"/>
+      <c r="P36" s="50"/>
     </row>
     <row r="37" spans="4:16">
       <c r="D37" t="str">
         <v>Coco Vanilla</v>
       </c>
-      <c r="P37" s="52" t="s">
+      <c r="P37" s="50" t="s">
         <v>324</v>
       </c>
     </row>
@@ -11270,13 +11276,13 @@
       <c r="D38" t="str">
         <v>Honey Honey</v>
       </c>
-      <c r="P38" s="52"/>
+      <c r="P38" s="50"/>
     </row>
     <row r="39" spans="4:16">
       <c r="D39" t="str">
         <v>Cinnamon Swirl</v>
       </c>
-      <c r="P39" s="52" t="s">
+      <c r="P39" s="50" t="s">
         <v>332</v>
       </c>
     </row>
@@ -11284,13 +11290,13 @@
       <c r="D40" t="str">
         <v>Apple &amp; Cinnamon</v>
       </c>
-      <c r="P40" s="52"/>
+      <c r="P40" s="50"/>
     </row>
     <row r="41" spans="4:16">
       <c r="D41" t="str">
         <v>Green Tea</v>
       </c>
-      <c r="P41" s="52" t="s">
+      <c r="P41" s="50" t="s">
         <v>330</v>
       </c>
     </row>
@@ -11298,13 +11304,13 @@
       <c r="D42" t="str">
         <v>Green Apple</v>
       </c>
-      <c r="P42" s="52"/>
+      <c r="P42" s="50"/>
     </row>
     <row r="43" spans="4:16">
       <c r="D43" t="str">
         <v>Golden Night</v>
       </c>
-      <c r="P43" s="52" t="s">
+      <c r="P43" s="50" t="s">
         <v>334</v>
       </c>
     </row>
@@ -11312,13 +11318,13 @@
       <c r="D44" t="str">
         <v>Rred Fruits</v>
       </c>
-      <c r="P44" s="52"/>
+      <c r="P44" s="50"/>
     </row>
     <row r="45" spans="4:16">
       <c r="D45" t="str">
         <v>Strawberry</v>
       </c>
-      <c r="P45" s="52" t="s">
+      <c r="P45" s="50" t="s">
         <v>335</v>
       </c>
     </row>
@@ -11331,7 +11337,7 @@
       <c r="D47" t="str">
         <v>Chocolate</v>
       </c>
-      <c r="P47" s="51" t="s">
+      <c r="P47" s="49" t="s">
         <v>546</v>
       </c>
     </row>
@@ -11339,13 +11345,13 @@
       <c r="D48" t="str">
         <v>Capuccino Lover</v>
       </c>
-      <c r="P48" s="52"/>
+      <c r="P48" s="50"/>
     </row>
     <row r="49" spans="4:16">
       <c r="D49" t="str">
         <v>Moccaccino Lover</v>
       </c>
-      <c r="P49" s="52" t="s">
+      <c r="P49" s="50" t="s">
         <v>344</v>
       </c>
     </row>
@@ -11353,13 +11359,13 @@
       <c r="D50" t="str">
         <v>Pets &amp; Animals</v>
       </c>
-      <c r="P50" s="52"/>
+      <c r="P50" s="50"/>
     </row>
     <row r="51" spans="4:16">
       <c r="D51" t="str">
         <v>Bubble Candles</v>
       </c>
-      <c r="P51" s="52" t="s">
+      <c r="P51" s="50" t="s">
         <v>365</v>
       </c>
     </row>
@@ -11367,13 +11373,13 @@
       <c r="D52" t="str">
         <v>Lucky Life</v>
       </c>
-      <c r="P52" s="52"/>
+      <c r="P52" s="50"/>
     </row>
     <row r="53" spans="4:16">
       <c r="D53" t="str">
         <v>Miscellaneous</v>
       </c>
-      <c r="P53" s="52" t="s">
+      <c r="P53" s="50" t="s">
         <v>347</v>
       </c>
     </row>
@@ -11381,13 +11387,13 @@
       <c r="D54" t="str">
         <v xml:space="preserve">Teddy Bears </v>
       </c>
-      <c r="P54" s="52"/>
+      <c r="P54" s="50"/>
     </row>
     <row r="55" spans="4:16">
       <c r="D55" t="str">
         <v>Rainbows</v>
       </c>
-      <c r="P55" s="52" t="s">
+      <c r="P55" s="50" t="s">
         <v>340</v>
       </c>
     </row>
@@ -11395,13 +11401,13 @@
       <c r="D56" t="str">
         <v>Family &amp; Friends</v>
       </c>
-      <c r="P56" s="52"/>
+      <c r="P56" s="50"/>
     </row>
     <row r="57" spans="4:16">
       <c r="D57" t="str">
         <v xml:space="preserve">Hearts </v>
       </c>
-      <c r="P57" s="52" t="s">
+      <c r="P57" s="50" t="s">
         <v>310</v>
       </c>
     </row>
@@ -11409,13 +11415,13 @@
       <c r="D58" t="str">
         <v>Pillar  &amp; Taper Candles</v>
       </c>
-      <c r="P58" s="52"/>
+      <c r="P58" s="50"/>
     </row>
     <row r="59" spans="4:16">
       <c r="D59" t="str">
         <v>Halloween</v>
       </c>
-      <c r="P59" s="52" t="s">
+      <c r="P59" s="50" t="s">
         <v>311</v>
       </c>
     </row>
@@ -11423,155 +11429,156 @@
       <c r="D60" t="str">
         <v>Christmas Time</v>
       </c>
-      <c r="P60" s="52"/>
+      <c r="P60" s="50"/>
     </row>
     <row r="61" spans="4:16">
       <c r="D61" t="str">
         <v>Flowers</v>
       </c>
-      <c r="P61" s="52" t="s">
+      <c r="P61" s="50" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="62" spans="4:16">
-      <c r="P62" s="52"/>
+      <c r="P62" s="50"/>
     </row>
     <row r="63" spans="4:16">
-      <c r="P63" s="52" t="s">
+      <c r="P63" s="50" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="64" spans="4:16">
-      <c r="P64" s="52"/>
+      <c r="P64" s="50"/>
     </row>
     <row r="65" spans="16:16">
-      <c r="P65" s="52" t="s">
+      <c r="P65" s="50" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="67" spans="16:16" ht="15.6">
-      <c r="P67" s="51" t="s">
+      <c r="P67" s="49" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="68" spans="16:16">
-      <c r="P68" s="52"/>
+      <c r="P68" s="50"/>
     </row>
     <row r="69" spans="16:16">
-      <c r="P69" s="52" t="s">
+      <c r="P69" s="50" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="70" spans="16:16">
-      <c r="P70" s="52"/>
+      <c r="P70" s="50"/>
     </row>
     <row r="71" spans="16:16">
-      <c r="P71" s="52" t="s">
+      <c r="P71" s="50" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="72" spans="16:16">
-      <c r="P72" s="52"/>
+      <c r="P72" s="50"/>
     </row>
     <row r="73" spans="16:16">
-      <c r="P73" s="52" t="s">
+      <c r="P73" s="50" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="74" spans="16:16">
-      <c r="P74" s="52"/>
+      <c r="P74" s="50"/>
     </row>
     <row r="75" spans="16:16">
-      <c r="P75" s="52" t="s">
+      <c r="P75" s="50" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="76" spans="16:16">
-      <c r="P76" s="52"/>
+      <c r="P76" s="50"/>
     </row>
     <row r="77" spans="16:16">
-      <c r="P77" s="52" t="s">
+      <c r="P77" s="50" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="78" spans="16:16">
-      <c r="P78" s="52"/>
+      <c r="P78" s="50"/>
     </row>
     <row r="79" spans="16:16">
-      <c r="P79" s="52" t="s">
+      <c r="P79" s="50" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="80" spans="16:16">
-      <c r="P80" s="52"/>
+      <c r="P80" s="50"/>
     </row>
     <row r="81" spans="16:16">
-      <c r="P81" s="52" t="s">
+      <c r="P81" s="50" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="82" spans="16:16">
-      <c r="P82" s="52"/>
+      <c r="P82" s="50"/>
     </row>
     <row r="83" spans="16:16">
-      <c r="P83" s="52" t="s">
+      <c r="P83" s="50" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="84" spans="16:16">
-      <c r="P84" s="52"/>
+      <c r="P84" s="50"/>
     </row>
     <row r="85" spans="16:16">
-      <c r="P85" s="52" t="s">
+      <c r="P85" s="50" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="86" spans="16:16">
-      <c r="P86" s="52"/>
+      <c r="P86" s="50"/>
     </row>
     <row r="87" spans="16:16">
-      <c r="P87" s="52" t="s">
+      <c r="P87" s="50" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="88" spans="16:16">
-      <c r="P88" s="52"/>
+      <c r="P88" s="50"/>
     </row>
     <row r="89" spans="16:16">
-      <c r="P89" s="52" t="s">
+      <c r="P89" s="50" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="90" spans="16:16">
-      <c r="P90" s="52"/>
+      <c r="P90" s="50"/>
     </row>
     <row r="91" spans="16:16">
-      <c r="P91" s="52" t="s">
+      <c r="P91" s="50" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="93" spans="16:16" ht="15.6">
-      <c r="P93" s="51" t="s">
+      <c r="P93" s="49" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="94" spans="16:16">
-      <c r="P94" s="52"/>
+      <c r="P94" s="50"/>
     </row>
     <row r="95" spans="16:16">
-      <c r="P95" s="52" t="s">
+      <c r="P95" s="50" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="96" spans="16:16">
-      <c r="P96" s="52"/>
+      <c r="P96" s="50"/>
     </row>
     <row r="97" spans="16:16">
-      <c r="P97" s="52" t="s">
+      <c r="P97" s="50" t="s">
         <v>333</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G61" xr:uid="{19C63E3B-0038-4417-BE29-7F9029D8CDB7}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11601,10 +11608,10 @@
   <sheetData>
     <row r="2" spans="1:2" ht="15" thickBot="1"/>
     <row r="3" spans="1:2">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="52"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">

</xml_diff>